<commit_message>
added @export to documentation, used dplyr to make DSR function work with grouped area data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Numerator</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>UL998CL</t>
+  </si>
+  <si>
+    <t>LL95CI</t>
+  </si>
+  <si>
+    <t>UL95CI</t>
+  </si>
+  <si>
+    <t>LL998CI</t>
+  </si>
+  <si>
+    <t>UL998CI</t>
   </si>
 </sst>
 </file>
@@ -690,7 +702,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WIP amends to quantiles, quantiles test script, proportions
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEstatmethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861B0C7-1F9C-4E2D-8FED-0BE2DE86A9D9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Prop" sheetId="3" r:id="rId1"/>
+    <sheet name="testdata_Prop_g" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
   <si>
     <t>Numerator</t>
   </si>
@@ -98,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,11 +436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,4 +1613,326 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BDD4BF-DA3C-4E63-8E1A-0835ACE9078C}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A2,testdata_Prop!B$2:B$33)</f>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A2,testdata_Prop!C$2:C$33)</f>
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0.79837991089509919</v>
+      </c>
+      <c r="E2">
+        <v>0.79481805800067218</v>
+      </c>
+      <c r="F2">
+        <v>0.80189534317473543</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A3,testdata_Prop!B$2:B$33)</f>
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A3,testdata_Prop!C$2:C$33)</f>
+        <v>400</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <v>3.2597429837147258E-2</v>
+      </c>
+      <c r="F3">
+        <v>7.5963635063719587E-2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A4,testdata_Prop!B$2:B$33)</f>
+        <v>80</v>
+      </c>
+      <c r="C4">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A4,testdata_Prop!C$2:C$33)</f>
+        <v>400</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>0.16373705973387687</v>
+      </c>
+      <c r="F4">
+        <v>0.24197031686670104</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A5,testdata_Prop!B$2:B$33)</f>
+        <v>260</v>
+      </c>
+      <c r="C5">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A5,testdata_Prop!C$2:C$33)</f>
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <v>0.65</v>
+      </c>
+      <c r="E5">
+        <v>0.60203196070747378</v>
+      </c>
+      <c r="F5">
+        <v>0.69511435099223728</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A6,testdata_Prop!B$2:B$33)</f>
+        <v>39424</v>
+      </c>
+      <c r="C6">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A6,testdata_Prop!C$2:C$33)</f>
+        <v>49380</v>
+      </c>
+      <c r="D6">
+        <v>0.79837991089509919</v>
+      </c>
+      <c r="E6">
+        <v>0.79481805800067218</v>
+      </c>
+      <c r="F6">
+        <v>0.80189534317473543</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A7,testdata_Prop!B$2:B$33)</f>
+        <v>31105824</v>
+      </c>
+      <c r="C7">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A7,testdata_Prop!C$2:C$33)</f>
+        <v>30257346708</v>
+      </c>
+      <c r="D7">
+        <v>1.0280420256339154E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.0276809995663644E-3</v>
+      </c>
+      <c r="F7">
+        <v>1.0284031783999669E-3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A8,testdata_Prop!B$2:B$33)</f>
+        <v>888</v>
+      </c>
+      <c r="C8">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A8,testdata_Prop!C$2:C$33)</f>
+        <v>12860</v>
+      </c>
+      <c r="D8">
+        <v>6.9051321928460335E-2</v>
+      </c>
+      <c r="E8">
+        <v>6.4796737148613115E-2</v>
+      </c>
+      <c r="F8">
+        <v>7.3563290415335325E-2</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A9,testdata_Prop!B$2:B$33)</f>
+        <v>3996</v>
+      </c>
+      <c r="C9">
+        <f>SUMIF(testdata_Prop!$A$2:$A$33,testdata_Prop_g!$A9,testdata_Prop!C$2:C$33)</f>
+        <v>13824</v>
+      </c>
+      <c r="D9">
+        <v>0.2890625</v>
+      </c>
+      <c r="E9">
+        <v>0.28156503717401421</v>
+      </c>
+      <c r="F9">
+        <v>0.29667716227788915</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Amended wilson, byars, proportion and rate function so can handle NA values - complete and NA testdata included. Sorted testdata for new grouped output in proportion and rate functions.  Amended proportion and rate function example code to include grouped dfs and NA values.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861B0C7-1F9C-4E2D-8FED-0BE2DE86A9D9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A7C0FD-30EC-4BCC-8FB4-7EE77AC75880}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Prop" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="26">
   <si>
     <t>Numerator</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Area9</t>
+  </si>
+  <si>
+    <t>Area10</t>
+  </si>
+  <si>
+    <t>Area11</t>
   </si>
 </sst>
 </file>
@@ -150,13 +159,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,6 +1619,63 @@
         <v>100</v>
       </c>
     </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2">
+        <v>100</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1617,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BDD4BF-DA3C-4E63-8E1A-0835ACE9078C}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,6 +1999,63 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tidying up to prep for devtools checks - documentation updated.  phe_proportion and phe_rate amended for grouped data frames.  phe_quantiles test script finalised.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A7C0FD-30EC-4BCC-8FB4-7EE77AC75880}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55C4B3E-C1FA-42EC-AA46-F1D04B34741C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Prop" sheetId="3" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BDD4BF-DA3C-4E63-8E1A-0835ACE9078C}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,13 +1740,13 @@
         <v>400</v>
       </c>
       <c r="D2">
-        <v>0.79837991089509919</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.79481805800067218</v>
+        <v>3.8954837949909914E-3</v>
       </c>
       <c r="F2">
-        <v>0.80189534317473543</v>
+        <v>2.5426564652619579E-2</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Replaced phe_proportion argument percentage with multiplier.  Need to sort warning in expect_equal test and make note in news file re back compatibility.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55C4B3E-C1FA-42EC-AA46-F1D04B34741C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E8F5A7-C074-496D-AFC7-3696017BFC8F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Prop" sheetId="3" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>proportion</t>
-  </si>
-  <si>
     <t>percentage</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Area11</t>
+  </si>
+  <si>
+    <t>proportion of 1</t>
   </si>
 </sst>
 </file>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,8 @@
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="5" customWidth="1"/>
-    <col min="8" max="10" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -478,13 +479,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -496,7 +497,7 @@
         <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -522,13 +523,13 @@
         <v>5.4486196178705294E-2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -557,13 +558,13 @@
         <v>0.11175046923191911</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -592,13 +593,13 @@
         <v>0.28882916559315885</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
@@ -627,13 +628,13 @@
         <v>0.73635751756902468</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -662,13 +663,13 @@
         <v>0.80536400736149094</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
@@ -697,13 +698,13 @@
         <v>1.0287644578977231E-3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -732,13 +733,13 @@
         <v>7.8339566813836331E-2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2">
         <v>1</v>
@@ -767,13 +768,13 @@
         <v>0.30440389662818057</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -802,13 +803,13 @@
         <v>5.4486196178705297</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="2">
         <v>100</v>
@@ -837,13 +838,13 @@
         <v>11.175046923191911</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="2">
         <v>100</v>
@@ -872,13 +873,13 @@
         <v>28.882916559315884</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" s="2">
         <v>100</v>
@@ -907,13 +908,13 @@
         <v>73.635751756902465</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" s="2">
         <v>100</v>
@@ -942,13 +943,13 @@
         <v>80.536400736149091</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" s="2">
         <v>100</v>
@@ -977,13 +978,13 @@
         <v>0.10287644578977231</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" s="2">
         <v>100</v>
@@ -1012,13 +1013,13 @@
         <v>7.8339566813836328</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16" s="2">
         <v>100</v>
@@ -1047,13 +1048,13 @@
         <v>30.440389662818056</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" s="2">
         <v>100</v>
@@ -1082,13 +1083,13 @@
         <v>0.10455445283705821</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -1117,13 +1118,13 @@
         <v>0.16458852282596442</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -1152,13 +1153,13 @@
         <v>0.3471109417008601</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -1187,13 +1188,13 @@
         <v>0.77835406140896968</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
@@ -1222,13 +1223,13 @@
         <v>0.80930614125896261</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -1257,13 +1258,13 @@
         <v>1.0291812992698397E-3</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
@@ -1292,13 +1293,13 @@
         <v>8.4184141852701344E-2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J24" s="2">
         <v>1</v>
@@ -1327,13 +1328,13 @@
         <v>0.31344754492799848</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" s="2">
         <v>1</v>
@@ -1362,13 +1363,13 @@
         <v>10.455445283705821</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J26" s="2">
         <v>100</v>
@@ -1397,13 +1398,13 @@
         <v>16.458852282596443</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J27" s="2">
         <v>100</v>
@@ -1432,13 +1433,13 @@
         <v>34.711094170086007</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J28" s="2">
         <v>100</v>
@@ -1467,13 +1468,13 @@
         <v>77.835406140896964</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J29" s="2">
         <v>100</v>
@@ -1502,13 +1503,13 @@
         <v>80.930614125896255</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J30" s="2">
         <v>100</v>
@@ -1537,13 +1538,13 @@
         <v>0.10291812992698397</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J31" s="2">
         <v>100</v>
@@ -1572,13 +1573,13 @@
         <v>8.4184141852701337</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" s="2">
         <v>100</v>
@@ -1607,13 +1608,13 @@
         <v>31.344754492799847</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J33" s="2">
         <v>100</v>
@@ -1621,19 +1622,19 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2">
         <v>100</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J34" s="2">
         <v>1</v>
@@ -1641,19 +1642,19 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35">
         <v>10</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -1661,16 +1662,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -1686,13 +1687,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BDD4BF-DA3C-4E63-8E1A-0835ACE9078C}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1706,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -1724,7 +1726,7 @@
         <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1749,13 +1751,13 @@
         <v>2.5426564652619579E-2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -1783,13 +1785,13 @@
         <v>7.5963635063719587E-2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -1817,13 +1819,13 @@
         <v>0.24197031686670104</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
@@ -1851,13 +1853,13 @@
         <v>0.69511435099223728</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1885,13 +1887,13 @@
         <v>0.80189534317473543</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
@@ -1919,13 +1921,13 @@
         <v>1.0284031783999669E-3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1953,13 +1955,13 @@
         <v>7.3563290415335325E-2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2">
         <v>1</v>
@@ -1987,13 +1989,13 @@
         <v>0.29667716227788915</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -2001,19 +2003,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -2021,19 +2023,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -2041,16 +2043,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12">
         <v>1</v>

</xml_diff>

<commit_message>
Actioned PF Documentation comments and amended test data to try to resolve testing issues on non-windows platforms.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Proportion.xlsx
+++ b/tests/testthat/testdata_Proportion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E8F5A7-C074-496D-AFC7-3696017BFC8F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C2C942-C723-44C0-B302-75715A26BDF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Prop" sheetId="3" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>Area9</t>
-  </si>
-  <si>
     <t>Area10</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>proportion of 1</t>
+  </si>
+  <si>
+    <t>Area09</t>
   </si>
 </sst>
 </file>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
@@ -561,7 +561,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
@@ -596,7 +596,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
@@ -631,7 +631,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>15</v>
@@ -666,7 +666,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>15</v>
@@ -736,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>15</v>
@@ -771,7 +771,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>15</v>
@@ -1086,7 +1086,7 @@
         <v>20</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>15</v>
@@ -1121,7 +1121,7 @@
         <v>20</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>15</v>
@@ -1156,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>15</v>
@@ -1191,7 +1191,7 @@
         <v>20</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>15</v>
@@ -1226,7 +1226,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>15</v>
@@ -1261,7 +1261,7 @@
         <v>20</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>15</v>
@@ -1296,7 +1296,7 @@
         <v>20</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>15</v>
@@ -1331,7 +1331,7 @@
         <v>20</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>15</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2">
         <v>100</v>
@@ -1631,7 +1631,7 @@
         <v>19</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>15</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>10</v>
@@ -1651,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I35" t="s">
         <v>15</v>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" t="s">
         <v>15</v>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BDD4BF-DA3C-4E63-8E1A-0835ACE9078C}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
@@ -1788,7 +1788,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
@@ -1822,7 +1822,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
@@ -1856,7 +1856,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>15</v>
@@ -1890,7 +1890,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
@@ -1924,7 +1924,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>15</v>
@@ -1958,7 +1958,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>15</v>
@@ -1992,7 +1992,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>15</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -2012,7 +2012,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -2032,7 +2032,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" t="s">
         <v>15</v>
@@ -2043,13 +2043,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
         <v>15</v>

</xml_diff>